<commit_message>
adding alkalinity script from Steeve and Fred up-to-date
</commit_message>
<xml_diff>
--- a/Data/Spring_2023/Transplants/Alkalinity/BenthFun_Summary.xlsx
+++ b/Data/Spring_2023/Transplants/Alkalinity/BenthFun_Summary.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santella-SZN\Desktop\Total_Alkalinity\ischia_alkalinity_data\titrator_backup\2023\BenthFun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Desktop/Total_Alkalinity/ischia_alkalinity_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9AC3A2-B0CA-684A-B498-E9AF22C8EA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="161">
   <si>
     <t>Operator</t>
   </si>
@@ -318,12 +326,201 @@
   </si>
   <si>
     <t>ALK batch</t>
+  </si>
+  <si>
+    <t>CRM3</t>
+  </si>
+  <si>
+    <t>T1_t0_ELOW_blank_01a</t>
+  </si>
+  <si>
+    <t>T1_t0_ELOW_blank_01b</t>
+  </si>
+  <si>
+    <t>T1_t0_ELOW_blank_01c</t>
+  </si>
+  <si>
+    <t>T1_t0_ELOW_blank_02a</t>
+  </si>
+  <si>
+    <t>T1_t0_ELOW_blank_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_01a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_01b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_01c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_02a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_02c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_03a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_03b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_03c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_01a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_01b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_01c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_04a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_04b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_04c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_05a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_05b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_06a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_06b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_tile_06c</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_02a</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_ELOW_blank_02c</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_01a</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_01b</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_01c</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_02a</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_01a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_01b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_02a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_02c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_03a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_03b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_01a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_01b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_01c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_04a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_04b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_05a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_05b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_06a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_06b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_06c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_02a</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_02b</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_02c</t>
+  </si>
+  <si>
+    <t>T1_t0_LOW_blank_02c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_05c</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_01c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_04c</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_blank_02d</t>
+  </si>
+  <si>
+    <t>T1_t1_LOW_tile_06d</t>
+  </si>
+  <si>
+    <t>bottle fell and broke</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -468,9 +665,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,32 +976,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M148" sqref="M148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="15" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -811,7 +1039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -853,7 +1081,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
@@ -879,7 +1107,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
@@ -914,7 +1142,7 @@
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -940,7 +1168,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -966,7 +1194,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -1001,7 +1229,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -1027,7 +1255,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1281,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1316,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1341,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1366,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -1172,7 +1400,7 @@
         <v>2592.88</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +1426,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1461,7 @@
       </c>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
@@ -1258,7 +1486,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1520,7 @@
         <v>2621.1999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -1317,7 +1545,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -1342,7 +1570,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +1604,7 @@
         <v>2553.7799999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -1401,7 +1629,7 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
@@ -1426,7 +1654,7 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
@@ -1460,7 +1688,7 @@
         <v>2531.04</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
@@ -1485,7 +1713,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
@@ -1519,7 +1747,7 @@
         <v>2487.5749999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
@@ -1544,7 +1772,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
@@ -1569,7 +1797,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
@@ -1594,7 +1822,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
@@ -1628,7 +1856,7 @@
         <v>2606.9649999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
@@ -1653,7 +1881,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +1906,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1689,7 +1917,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
@@ -1731,7 +1959,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
@@ -1756,7 +1984,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
@@ -1788,7 +2016,7 @@
         <v>2658.0949999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
@@ -1808,7 +2036,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
@@ -1840,7 +2068,7 @@
         <v>2655.7449999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
@@ -1860,7 +2088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -1880,7 +2108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>11</v>
       </c>
@@ -1912,7 +2140,7 @@
         <v>2591.3400000000006</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
@@ -1932,7 +2160,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>11</v>
       </c>
@@ -1952,7 +2180,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>11</v>
       </c>
@@ -1972,7 +2200,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
@@ -2004,7 +2232,7 @@
         <v>2576.5950000000007</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
@@ -2024,7 +2252,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
@@ -2044,7 +2272,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>11</v>
       </c>
@@ -2064,7 +2292,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2324,7 @@
         <v>2579.6250000000005</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>11</v>
       </c>
@@ -2116,7 +2344,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2364,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>11</v>
       </c>
@@ -2168,7 +2396,7 @@
         <v>2650.0800000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>11</v>
       </c>
@@ -2188,7 +2416,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>11</v>
       </c>
@@ -2220,7 +2448,7 @@
         <v>2556.6850000000004</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>11</v>
       </c>
@@ -2240,7 +2468,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>11</v>
       </c>
@@ -2260,7 +2488,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>11</v>
       </c>
@@ -2292,7 +2520,7 @@
         <v>2532.8100000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2540,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>11</v>
       </c>
@@ -2344,7 +2572,7 @@
         <v>2540.77</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>11</v>
       </c>
@@ -2364,7 +2592,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>11</v>
       </c>
@@ -2396,7 +2624,7 @@
         <v>2633.7750000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>11</v>
       </c>
@@ -2416,7 +2644,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>11</v>
       </c>
@@ -2458,7 +2686,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>11</v>
       </c>
@@ -2483,7 +2711,7 @@
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>11</v>
       </c>
@@ -2515,7 +2743,7 @@
         <v>2674.7000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>11</v>
       </c>
@@ -2535,7 +2763,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>11</v>
       </c>
@@ -2555,7 +2783,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>11</v>
       </c>
@@ -2587,7 +2815,7 @@
         <v>2650.1000000000004</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>11</v>
       </c>
@@ -2607,7 +2835,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>11</v>
       </c>
@@ -2627,7 +2855,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>11</v>
       </c>
@@ -2659,7 +2887,7 @@
         <v>2343.2800000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>11</v>
       </c>
@@ -2679,7 +2907,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>11</v>
       </c>
@@ -2711,7 +2939,7 @@
         <v>2642.0000000000005</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>11</v>
       </c>
@@ -2731,7 +2959,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
         <v>11</v>
       </c>
@@ -2763,7 +2991,7 @@
         <v>2620.7650000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>11</v>
       </c>
@@ -2783,7 +3011,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>11</v>
       </c>
@@ -2815,7 +3043,7 @@
         <v>2663.0850000000005</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>11</v>
       </c>
@@ -2835,7 +3063,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>11</v>
       </c>
@@ -2855,7 +3083,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>11</v>
       </c>
@@ -2887,7 +3115,7 @@
         <v>2576.9600000000005</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>11</v>
       </c>
@@ -2907,7 +3135,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>11</v>
       </c>
@@ -2927,7 +3155,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
         <v>11</v>
       </c>
@@ -2959,7 +3187,7 @@
         <v>2584.4350000000004</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>11</v>
       </c>
@@ -2979,7 +3207,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>11</v>
       </c>
@@ -2999,7 +3227,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
         <v>11</v>
       </c>
@@ -3031,7 +3259,7 @@
         <v>2557.5100000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
         <v>11</v>
       </c>
@@ -3051,7 +3279,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
         <v>11</v>
       </c>
@@ -3071,7 +3299,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>11</v>
       </c>
@@ -3103,7 +3331,7 @@
         <v>2654.3750000000005</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
         <v>11</v>
       </c>
@@ -3121,6 +3349,2394 @@
       </c>
       <c r="F90" s="16" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B92" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="5">
+        <v>48.55</v>
+      </c>
+      <c r="E92" s="5">
+        <v>2252.11</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G92" s="12">
+        <f>AVERAGE(E92,E94)</f>
+        <v>2251.09</v>
+      </c>
+      <c r="H92" s="13">
+        <f>STDEV(E92,E94)</f>
+        <v>1.4424978336205312</v>
+      </c>
+      <c r="I92" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J92" s="4">
+        <f>I92-G92</f>
+        <v>-24.650000000000091</v>
+      </c>
+      <c r="K92" s="5">
+        <f>G92+J92</f>
+        <v>2226.44</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="5">
+        <v>47.52</v>
+      </c>
+      <c r="E93" s="14">
+        <v>2245.7600000000002</v>
+      </c>
+      <c r="F93" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="5">
+        <v>48.34</v>
+      </c>
+      <c r="E94" s="5">
+        <v>2250.0700000000002</v>
+      </c>
+      <c r="F94" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="5">
+        <v>51.96</v>
+      </c>
+      <c r="E95" s="5">
+        <v>2603.67</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G95" s="13">
+        <f>AVERAGE(E95,E97)</f>
+        <v>2602.0950000000003</v>
+      </c>
+      <c r="H95" s="18">
+        <f>STDEV(E95,E97)</f>
+        <v>2.2273863607376891</v>
+      </c>
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5">
+        <f>G95+$J$92</f>
+        <v>2577.4450000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96" s="5">
+        <v>49.08</v>
+      </c>
+      <c r="E96" s="14">
+        <v>2586.33</v>
+      </c>
+      <c r="F96" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" s="5">
+        <v>50.05</v>
+      </c>
+      <c r="E97" s="5">
+        <v>2600.52</v>
+      </c>
+      <c r="F97" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="5">
+        <v>51.59</v>
+      </c>
+      <c r="E98" s="5">
+        <v>2578.59</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G98" s="13">
+        <f>AVERAGE(E98:E99)</f>
+        <v>2579.4549999999999</v>
+      </c>
+      <c r="H98" s="18">
+        <f>STDEV(E98:E99)</f>
+        <v>1.22329473145274</v>
+      </c>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5">
+        <f>G98+$J$92</f>
+        <v>2554.8049999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="5">
+        <v>50.52</v>
+      </c>
+      <c r="E99" s="5">
+        <v>2580.3200000000002</v>
+      </c>
+      <c r="F99" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="5">
+        <v>51.8</v>
+      </c>
+      <c r="E100" s="14">
+        <v>3004.58</v>
+      </c>
+      <c r="F100" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G100" s="13">
+        <f>AVERAGE(E101:E102)</f>
+        <v>3027.23</v>
+      </c>
+      <c r="H100" s="18">
+        <f>STDEV(E101:E102)</f>
+        <v>2.390020920410608</v>
+      </c>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5">
+        <f>G100+$J$92</f>
+        <v>3002.58</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" s="5">
+        <v>51.36</v>
+      </c>
+      <c r="E101" s="5">
+        <v>3025.54</v>
+      </c>
+      <c r="F101" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="5">
+        <v>52.44</v>
+      </c>
+      <c r="E102" s="5">
+        <v>3028.92</v>
+      </c>
+      <c r="F102" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" s="5">
+        <v>49.3</v>
+      </c>
+      <c r="E103" s="5">
+        <v>3016.39</v>
+      </c>
+      <c r="F103" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G103" s="13">
+        <f>AVERAGE(E103,E105)</f>
+        <v>3014.8599999999997</v>
+      </c>
+      <c r="H103" s="18">
+        <f>STDEV(E103,E105)</f>
+        <v>2.1637467504307968</v>
+      </c>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5">
+        <f>G103+$J$92</f>
+        <v>2990.2099999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B104" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="5">
+        <v>51.02</v>
+      </c>
+      <c r="E104" s="14">
+        <v>2995.09</v>
+      </c>
+      <c r="F104" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B105" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" s="5">
+        <v>49.61</v>
+      </c>
+      <c r="E105" s="5">
+        <v>3013.33</v>
+      </c>
+      <c r="F105" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B106" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="5">
+        <v>52.32</v>
+      </c>
+      <c r="E106" s="14">
+        <v>3010.86</v>
+      </c>
+      <c r="F106" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G106" s="13">
+        <f>AVERAGE(E107:E108)</f>
+        <v>3001.3</v>
+      </c>
+      <c r="H106" s="18">
+        <f>STDEV(E107:E108)</f>
+        <v>4.879036790187242</v>
+      </c>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5">
+        <f>G106+$J$92</f>
+        <v>2976.65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B107" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="5">
+        <v>49.03</v>
+      </c>
+      <c r="E107" s="5">
+        <v>2997.85</v>
+      </c>
+      <c r="F107" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" s="5">
+        <v>49.61</v>
+      </c>
+      <c r="E108" s="5">
+        <v>3004.75</v>
+      </c>
+      <c r="F108" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B109" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="5">
+        <v>47.83</v>
+      </c>
+      <c r="E109" s="14">
+        <v>2696.29</v>
+      </c>
+      <c r="F109" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G109" s="13">
+        <f>AVERAGE(E110:E111)</f>
+        <v>2682.9300000000003</v>
+      </c>
+      <c r="H109" s="18">
+        <f>STDEV(E110:E111)</f>
+        <v>0.42426406871186417</v>
+      </c>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5">
+        <f>G109+$J$92</f>
+        <v>2658.28</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B110" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="5">
+        <v>49.41</v>
+      </c>
+      <c r="E110" s="5">
+        <v>2683.23</v>
+      </c>
+      <c r="F110" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B111" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="5">
+        <v>50.51</v>
+      </c>
+      <c r="E111" s="5">
+        <v>2682.63</v>
+      </c>
+      <c r="F111" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B112" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D112" s="5">
+        <v>49.35</v>
+      </c>
+      <c r="E112" s="14">
+        <v>2673.54</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G112" s="13">
+        <f>AVERAGE(E113:E114)</f>
+        <v>2666.21</v>
+      </c>
+      <c r="H112" s="18">
+        <f>STDEV(E113:E114)</f>
+        <v>3.3658282784481206</v>
+      </c>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5">
+        <f>G112+$J$92</f>
+        <v>2641.56</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B113" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="5">
+        <v>51.51</v>
+      </c>
+      <c r="E113" s="5">
+        <v>2663.83</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B114" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="5">
+        <v>51.15</v>
+      </c>
+      <c r="E114" s="5">
+        <v>2668.59</v>
+      </c>
+      <c r="F114" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B115" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="5">
+        <v>52.36</v>
+      </c>
+      <c r="E115" s="5">
+        <v>2674.22</v>
+      </c>
+      <c r="F115" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G115" s="13">
+        <f>AVERAGE(E115:E116)</f>
+        <v>2676.22</v>
+      </c>
+      <c r="H115" s="18">
+        <f>STDEV(E115:E116)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5">
+        <f>G115+$J$92</f>
+        <v>2651.5699999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="5">
+        <v>50.56</v>
+      </c>
+      <c r="E116" s="5">
+        <v>2678.22</v>
+      </c>
+      <c r="F116" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B117" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" s="5">
+        <v>49.76</v>
+      </c>
+      <c r="E117" s="5">
+        <v>2672.81</v>
+      </c>
+      <c r="F117" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G117" s="13">
+        <f>AVERAGE(E117,E119)</f>
+        <v>2671.2349999999997</v>
+      </c>
+      <c r="H117" s="18">
+        <f>STDEV(E117,E119)</f>
+        <v>2.2273863607376891</v>
+      </c>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+      <c r="K117" s="5">
+        <f>G117+$J$92</f>
+        <v>2646.5849999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="5">
+        <v>49.93</v>
+      </c>
+      <c r="E118" s="14">
+        <v>2644.37</v>
+      </c>
+      <c r="F118" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119" s="15">
+        <v>50.21</v>
+      </c>
+      <c r="E119" s="5">
+        <v>2669.66</v>
+      </c>
+      <c r="F119" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B120" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" s="5">
+        <v>51.39</v>
+      </c>
+      <c r="E120" s="5">
+        <v>2602.8000000000002</v>
+      </c>
+      <c r="F120" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G120" s="13">
+        <f>AVERAGE(E120,E122)</f>
+        <v>2602.42</v>
+      </c>
+      <c r="H120" s="18">
+        <f>STDEV(E120,E122)</f>
+        <v>0.53740115370193042</v>
+      </c>
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="5">
+        <f>G120+$J$92</f>
+        <v>2577.77</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B121" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121" s="5">
+        <v>49.24</v>
+      </c>
+      <c r="E121" s="14">
+        <v>2621.53</v>
+      </c>
+      <c r="F121" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B122" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C122" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="5">
+        <v>48.74</v>
+      </c>
+      <c r="E122" s="5">
+        <v>2602.04</v>
+      </c>
+      <c r="F122" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A124" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" s="5">
+        <v>48.65</v>
+      </c>
+      <c r="E124" s="5">
+        <v>2243.71</v>
+      </c>
+      <c r="F124" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G124" s="12">
+        <f>AVERAGE(E124,E126)</f>
+        <v>2243.3900000000003</v>
+      </c>
+      <c r="H124" s="13">
+        <f>STDEV(E124,E126)</f>
+        <v>0.45254833995930038</v>
+      </c>
+      <c r="I124" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J124" s="4">
+        <f>I124-G124</f>
+        <v>-16.950000000000273</v>
+      </c>
+      <c r="K124" s="5">
+        <f>G124+J124</f>
+        <v>2226.44</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A125" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B125" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D125" s="5">
+        <v>52.32</v>
+      </c>
+      <c r="E125" s="14">
+        <v>2236.0300000000002</v>
+      </c>
+      <c r="F125" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D126" s="5">
+        <v>49.16</v>
+      </c>
+      <c r="E126" s="20">
+        <v>2243.0700000000002</v>
+      </c>
+      <c r="F126" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B127" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C127" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" s="5">
+        <v>50.06</v>
+      </c>
+      <c r="E127" s="14">
+        <v>2581.9299999999998</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G127" s="13">
+        <f>AVERAGE(E128,E129)</f>
+        <v>2560.4349999999999</v>
+      </c>
+      <c r="H127" s="18">
+        <f>STDEV(E128,E129)</f>
+        <v>1.3788582233136391</v>
+      </c>
+      <c r="I127" s="5"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="5">
+        <f>G127+$J$92</f>
+        <v>2535.7849999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B128" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C128" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D128" s="5">
+        <v>53.5</v>
+      </c>
+      <c r="E128" s="5">
+        <v>2559.46</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" s="5">
+        <v>49.18</v>
+      </c>
+      <c r="E129" s="5">
+        <v>2561.41</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B130" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C130" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" s="5">
+        <v>48.74</v>
+      </c>
+      <c r="E130" s="14">
+        <v>2581.9</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G130" s="13">
+        <f>AVERAGE(E131,E132)</f>
+        <v>2565.64</v>
+      </c>
+      <c r="H130" s="18">
+        <f>STDEV(E131,E132)</f>
+        <v>3.2102647865869001</v>
+      </c>
+      <c r="I130" s="5"/>
+      <c r="J130" s="5"/>
+      <c r="K130" s="5">
+        <f>G130+$J$92</f>
+        <v>2540.9899999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B131" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" s="5">
+        <v>48.46</v>
+      </c>
+      <c r="E131" s="5">
+        <v>2563.37</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B132" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C132" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D132" s="5">
+        <v>51.63</v>
+      </c>
+      <c r="E132" s="5">
+        <v>2567.91</v>
+      </c>
+      <c r="F132" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C133" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" s="5">
+        <v>49.69</v>
+      </c>
+      <c r="E133" s="5">
+        <v>2507.44</v>
+      </c>
+      <c r="F133" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G133" s="13">
+        <f>AVERAGE(E133,E134)</f>
+        <v>2509.4250000000002</v>
+      </c>
+      <c r="H133" s="18">
+        <f>STDEV(E133,E134)</f>
+        <v>2.8072139213104523</v>
+      </c>
+      <c r="I133" s="5"/>
+      <c r="J133" s="5"/>
+      <c r="K133" s="5">
+        <f>G133+$J$92</f>
+        <v>2484.7750000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B134" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C134" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="5">
+        <v>49.44</v>
+      </c>
+      <c r="E134" s="5">
+        <v>2511.41</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B135" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D135" s="5">
+        <v>50.55</v>
+      </c>
+      <c r="E135" s="14">
+        <v>2483.41</v>
+      </c>
+      <c r="F135" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G135" s="13">
+        <f>AVERAGE(E136,E137)</f>
+        <v>2508.37</v>
+      </c>
+      <c r="H135" s="18">
+        <f>STDEV(E136,E137)</f>
+        <v>2.036467529817334</v>
+      </c>
+      <c r="I135" s="5"/>
+      <c r="J135" s="5"/>
+      <c r="K135" s="5">
+        <f>G135+$J$92</f>
+        <v>2483.7199999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B136" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C136" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D136" s="5">
+        <v>47.44</v>
+      </c>
+      <c r="E136" s="5">
+        <v>2506.9299999999998</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B137" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D137" s="5">
+        <v>52.79</v>
+      </c>
+      <c r="E137" s="5">
+        <v>2509.81</v>
+      </c>
+      <c r="F137" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B138" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D138" s="5">
+        <v>48.3</v>
+      </c>
+      <c r="E138" s="5">
+        <v>2510.2199999999998</v>
+      </c>
+      <c r="F138" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G138" s="13">
+        <f>AVERAGE(E138,E139)</f>
+        <v>2513.62</v>
+      </c>
+      <c r="H138" s="18">
+        <f>STDEV(E138,E139)</f>
+        <v>4.8083261120686522</v>
+      </c>
+      <c r="I138" s="5"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="5">
+        <f>G138+$J$92</f>
+        <v>2488.9699999999998</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B139" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" s="5">
+        <v>48.44</v>
+      </c>
+      <c r="E139" s="5">
+        <v>2517.02</v>
+      </c>
+      <c r="F139" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B140" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140" s="5">
+        <v>49.14</v>
+      </c>
+      <c r="E140" s="14">
+        <v>2572.29</v>
+      </c>
+      <c r="F140" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G140" s="13">
+        <f>AVERAGE(E142,E141)</f>
+        <v>2555.61</v>
+      </c>
+      <c r="H140" s="18">
+        <f>STDEV(E142,E141)</f>
+        <v>3.5072496346853015</v>
+      </c>
+      <c r="I140" s="5"/>
+      <c r="J140" s="5"/>
+      <c r="K140" s="5">
+        <f>G140+$J$92</f>
+        <v>2530.96</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B141" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141" s="5">
+        <v>53.79</v>
+      </c>
+      <c r="E141" s="5">
+        <v>2558.09</v>
+      </c>
+      <c r="F141" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B142" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C142" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="5">
+        <v>48.08</v>
+      </c>
+      <c r="E142" s="5">
+        <v>2553.13</v>
+      </c>
+      <c r="F142" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B143" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C143" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" s="5">
+        <v>51.07</v>
+      </c>
+      <c r="E143" s="5">
+        <v>2490.64</v>
+      </c>
+      <c r="F143" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G143" s="13">
+        <f>AVERAGE(E143,E144)</f>
+        <v>2490.2249999999999</v>
+      </c>
+      <c r="H143" s="18">
+        <f>STDEV(E143,E144)</f>
+        <v>0.58689862838478302</v>
+      </c>
+      <c r="I143" s="5"/>
+      <c r="J143" s="5"/>
+      <c r="K143" s="5">
+        <f>G143+$J$92</f>
+        <v>2465.5749999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B144" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" s="5">
+        <v>48.78</v>
+      </c>
+      <c r="E144" s="5">
+        <v>2489.81</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A145" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B145" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C145" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F145" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G145" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H145" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="I145" s="5"/>
+      <c r="J145" s="5"/>
+      <c r="K145" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A146" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B146" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C146" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F146" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A147" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B147" s="10">
+        <v>45070</v>
+      </c>
+      <c r="C147" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F147" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A148" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B148" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D148" s="5">
+        <v>51.28</v>
+      </c>
+      <c r="E148" s="5">
+        <v>2508.1</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G148" s="13">
+        <f>AVERAGE(E148,E149)</f>
+        <v>2504.9749999999999</v>
+      </c>
+      <c r="H148" s="18">
+        <f>STDEV(E148,E149)</f>
+        <v>4.4194173824159222</v>
+      </c>
+      <c r="I148" s="5"/>
+      <c r="J148" s="5"/>
+      <c r="K148" s="5">
+        <f>G148+$J$124</f>
+        <v>2488.0249999999996</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A149" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B149" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C149" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D149" s="5">
+        <v>48.87</v>
+      </c>
+      <c r="E149" s="5">
+        <v>2501.85</v>
+      </c>
+      <c r="F149" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A150" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B150" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D150" s="5">
+        <v>50.15</v>
+      </c>
+      <c r="E150" s="14">
+        <v>2516.9699999999998</v>
+      </c>
+      <c r="F150" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A151" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D151" s="5">
+        <v>48.48</v>
+      </c>
+      <c r="E151" s="5">
+        <v>2563.36</v>
+      </c>
+      <c r="F151" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G151" s="13">
+        <f>AVERAGE(E151,E152)</f>
+        <v>2562.0500000000002</v>
+      </c>
+      <c r="H151" s="18">
+        <f>STDEV(E151,E152)</f>
+        <v>1.852619766708999</v>
+      </c>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="5">
+        <f>G151+$J$124</f>
+        <v>2545.1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A152" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C152" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D152" s="5">
+        <v>48.03</v>
+      </c>
+      <c r="E152" s="5">
+        <v>2560.7399999999998</v>
+      </c>
+      <c r="F152" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A153" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B153" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D153" s="5">
+        <v>48.88</v>
+      </c>
+      <c r="E153" s="14">
+        <v>2577.4</v>
+      </c>
+      <c r="F153" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A154" s="9"/>
+      <c r="B154" s="10"/>
+      <c r="C154" s="10"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="16"/>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A155" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B155" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C155" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D155" s="5">
+        <v>50.92</v>
+      </c>
+      <c r="E155" s="5">
+        <v>2235.3200000000002</v>
+      </c>
+      <c r="F155" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G155" s="12">
+        <f>AVERAGE(E155,E156)</f>
+        <v>2233.5550000000003</v>
+      </c>
+      <c r="H155" s="13">
+        <f>STDEV(E155:E156)</f>
+        <v>2.4960869375886543</v>
+      </c>
+      <c r="I155" s="3">
+        <v>2226.44</v>
+      </c>
+      <c r="J155" s="4">
+        <f>I155-G155</f>
+        <v>-7.1150000000002365</v>
+      </c>
+      <c r="K155" s="5">
+        <f>G155+J155</f>
+        <v>2226.44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A156" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B156" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C156" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D156" s="5">
+        <v>48.85</v>
+      </c>
+      <c r="E156" s="5">
+        <v>2231.79</v>
+      </c>
+      <c r="F156" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A157" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B157" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C157" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D157" s="5">
+        <v>49.29</v>
+      </c>
+      <c r="E157" s="14">
+        <v>2573.58</v>
+      </c>
+      <c r="F157" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G157" s="13">
+        <f>AVERAGE(E158:E159)</f>
+        <v>2559.56</v>
+      </c>
+      <c r="H157" s="18">
+        <f>STDEV(E158:E159)</f>
+        <v>3.2668333290817722</v>
+      </c>
+      <c r="I157" s="5"/>
+      <c r="J157" s="5"/>
+      <c r="K157" s="5">
+        <f>G157+$J$124</f>
+        <v>2542.6099999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A158" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B158" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C158" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158" s="5">
+        <v>50.59</v>
+      </c>
+      <c r="E158" s="5">
+        <v>2557.25</v>
+      </c>
+      <c r="F158" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A159" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B159" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C159" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="5">
+        <v>48.84</v>
+      </c>
+      <c r="E159" s="5">
+        <v>2561.87</v>
+      </c>
+      <c r="F159" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A160" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B160" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C160" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160" s="5">
+        <v>51.03</v>
+      </c>
+      <c r="E160" s="5">
+        <v>2571.7600000000002</v>
+      </c>
+      <c r="F160" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G160" s="13">
+        <f>AVERAGE(E160,E162)</f>
+        <v>2571.4499999999998</v>
+      </c>
+      <c r="H160" s="18">
+        <f>STDEV(E160,E162)</f>
+        <v>0.43840620433590383</v>
+      </c>
+      <c r="I160" s="5"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="5">
+        <f>G160+$J$124</f>
+        <v>2554.4999999999995</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A161" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B161" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D161" s="5">
+        <v>48.02</v>
+      </c>
+      <c r="E161" s="14">
+        <v>2641.36</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B162" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C162" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" s="5">
+        <v>51.38</v>
+      </c>
+      <c r="E162" s="5">
+        <v>2571.14</v>
+      </c>
+      <c r="F162" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A163" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B163" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D163" s="5">
+        <v>51.09</v>
+      </c>
+      <c r="E163" s="14">
+        <v>2509.6999999999998</v>
+      </c>
+      <c r="F163" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G163" s="13">
+        <f>AVERAGE(E164:E165)</f>
+        <v>2489.66</v>
+      </c>
+      <c r="H163" s="18">
+        <f>STDEV(E164:E165)</f>
+        <v>2.9698484809836927</v>
+      </c>
+      <c r="I163" s="5"/>
+      <c r="J163" s="5"/>
+      <c r="K163" s="5">
+        <f>G163+$J$124</f>
+        <v>2472.7099999999996</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A164" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C164" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D164" s="5">
+        <v>51.1</v>
+      </c>
+      <c r="E164" s="5">
+        <v>2491.7600000000002</v>
+      </c>
+      <c r="F164" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B165" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C165" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D165" s="5">
+        <v>52.26</v>
+      </c>
+      <c r="E165" s="5">
+        <v>2487.56</v>
+      </c>
+      <c r="F165" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A166" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B166" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C166" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D166" s="5">
+        <v>50.99</v>
+      </c>
+      <c r="E166" s="5">
+        <v>2526.11</v>
+      </c>
+      <c r="F166" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G166" s="13">
+        <f>AVERAGE(E166,E168)</f>
+        <v>2526.5600000000004</v>
+      </c>
+      <c r="H166" s="18">
+        <f>STDEV(E166,E168)</f>
+        <v>0.63639610306795713</v>
+      </c>
+      <c r="I166" s="5"/>
+      <c r="J166" s="5"/>
+      <c r="K166" s="5">
+        <f>G166+$J$124</f>
+        <v>2509.61</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A167" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C167" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D167" s="5">
+        <v>52.82</v>
+      </c>
+      <c r="E167" s="14">
+        <v>2520.5100000000002</v>
+      </c>
+      <c r="F167" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A168" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B168" s="10">
+        <v>45071</v>
+      </c>
+      <c r="C168" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D168" s="5">
+        <v>50.85</v>
+      </c>
+      <c r="E168" s="5">
+        <v>2527.0100000000002</v>
+      </c>
+      <c r="F168" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A169" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B169" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D169" s="5">
+        <v>50.49</v>
+      </c>
+      <c r="E169" s="5">
+        <v>2523.5</v>
+      </c>
+      <c r="F169" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G169" s="13">
+        <f>AVERAGE(E169:E170)</f>
+        <v>2521.355</v>
+      </c>
+      <c r="H169" s="18">
+        <f>STDEV(E169:E170)</f>
+        <v>3.0334880912902631</v>
+      </c>
+      <c r="I169" s="5"/>
+      <c r="J169" s="5"/>
+      <c r="K169" s="5">
+        <f>G169+$J$155</f>
+        <v>2514.2399999999998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A170" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B170" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D170" s="5">
+        <v>49.11</v>
+      </c>
+      <c r="E170" s="5">
+        <v>2519.21</v>
+      </c>
+      <c r="F170" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A171" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B171" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C171" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D171" s="5">
+        <v>52.28</v>
+      </c>
+      <c r="E171" s="5">
+        <v>2573.4699999999998</v>
+      </c>
+      <c r="F171" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G171" s="13">
+        <f>AVERAGE(E171,E173)</f>
+        <v>2574.1499999999996</v>
+      </c>
+      <c r="H171" s="18">
+        <f>STDEV(E171,E173)</f>
+        <v>0.96166522241379471</v>
+      </c>
+      <c r="I171" s="5"/>
+      <c r="J171" s="5"/>
+      <c r="K171" s="5">
+        <f>G171+$J$92</f>
+        <v>2549.4999999999995</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A172" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B172" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D172" s="5">
+        <v>50.12</v>
+      </c>
+      <c r="E172" s="14">
+        <v>2568.59</v>
+      </c>
+      <c r="F172" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A173" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B173" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C173" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D173" s="5">
+        <v>51.85</v>
+      </c>
+      <c r="E173" s="5">
+        <v>2574.83</v>
+      </c>
+      <c r="F173" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A174" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B174" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C174" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D174" s="5">
+        <v>50.5</v>
+      </c>
+      <c r="E174" s="5">
+        <v>2499.33</v>
+      </c>
+      <c r="F174" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G174" s="13">
+        <f>AVERAGE(E175:E176)</f>
+        <v>2508.4300000000003</v>
+      </c>
+      <c r="H174" s="18">
+        <f>STDEV(E175:E176)</f>
+        <v>3.2526911934580545</v>
+      </c>
+      <c r="I174" s="5"/>
+      <c r="J174" s="5"/>
+      <c r="K174" s="5">
+        <f>G174+$J$92</f>
+        <v>2483.7800000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A175" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B175" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C175" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D175" s="5">
+        <v>51.34</v>
+      </c>
+      <c r="E175" s="5">
+        <v>2510.73</v>
+      </c>
+      <c r="F175" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A176" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B176" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C176" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176" s="5">
+        <v>49.8</v>
+      </c>
+      <c r="E176" s="5">
+        <v>2506.13</v>
+      </c>
+      <c r="F176" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B177" s="25">
+        <v>45072</v>
+      </c>
+      <c r="C177" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D177" s="26">
+        <v>50.04</v>
+      </c>
+      <c r="E177" s="26">
+        <v>2464.9499999999998</v>
+      </c>
+      <c r="F177" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G177" s="13">
+        <f>AVERAGE(E177:E178)</f>
+        <v>2466.8249999999998</v>
+      </c>
+      <c r="H177" s="18">
+        <f>STDEV(E177:E178)</f>
+        <v>2.6516504294495533</v>
+      </c>
+      <c r="I177" s="26"/>
+      <c r="J177" s="26"/>
+      <c r="K177" s="26">
+        <f>G177+$J$92</f>
+        <v>2442.1749999999997</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B178" s="25">
+        <v>45072</v>
+      </c>
+      <c r="C178" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D178" s="26">
+        <v>48.8</v>
+      </c>
+      <c r="E178" s="26">
+        <v>2468.6999999999998</v>
+      </c>
+      <c r="F178" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G178" s="29"/>
+      <c r="H178" s="29"/>
+      <c r="I178" s="29"/>
+      <c r="J178" s="29"/>
+      <c r="K178" s="29"/>
+    </row>
+    <row r="179" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B179" s="25">
+        <v>45072</v>
+      </c>
+      <c r="C179" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D179" s="26">
+        <v>49.87</v>
+      </c>
+      <c r="E179" s="30">
+        <v>2431.39</v>
+      </c>
+      <c r="F179" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="G179" s="29"/>
+      <c r="H179" s="29"/>
+      <c r="I179" s="29"/>
+      <c r="J179" s="29"/>
+      <c r="K179" s="29"/>
+    </row>
+    <row r="180" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B180" s="25">
+        <v>45072</v>
+      </c>
+      <c r="C180" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D180" s="26">
+        <v>50.49</v>
+      </c>
+      <c r="E180" s="30">
+        <v>2513.27</v>
+      </c>
+      <c r="F180" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G180" s="13">
+        <f>AVERAGE(E181,E183)</f>
+        <v>2479.6350000000002</v>
+      </c>
+      <c r="H180" s="18">
+        <f>STDEV(E181,E183)</f>
+        <v>0.68589357775080961</v>
+      </c>
+      <c r="I180" s="5"/>
+      <c r="J180" s="5"/>
+      <c r="K180" s="5">
+        <f>G180+$J$92</f>
+        <v>2454.9850000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A181" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B181" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C181" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D181" s="5">
+        <v>49</v>
+      </c>
+      <c r="E181" s="5">
+        <v>2480.12</v>
+      </c>
+      <c r="F181" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="K181" s="1"/>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A182" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B182" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C182" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D182" s="22">
+        <v>49.92</v>
+      </c>
+      <c r="E182" s="14">
+        <v>2459.21</v>
+      </c>
+      <c r="F182" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A183" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B183" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C183" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D183" s="22">
+        <v>51.03</v>
+      </c>
+      <c r="E183" s="5">
+        <v>2479.15</v>
+      </c>
+      <c r="F183" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A184" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B184" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C184" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D184" s="22">
+        <v>52.74</v>
+      </c>
+      <c r="E184" s="14">
+        <v>2554.25</v>
+      </c>
+      <c r="F184" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G184" s="13">
+        <f>AVERAGE(E186:E187)</f>
+        <v>2569.605</v>
+      </c>
+      <c r="H184" s="18">
+        <f>STDEV(E186:E187)</f>
+        <v>4.0092954493277757</v>
+      </c>
+      <c r="I184" s="5"/>
+      <c r="J184" s="5"/>
+      <c r="K184" s="5">
+        <f>G184+$J$92</f>
+        <v>2544.9549999999999</v>
+      </c>
+      <c r="L184" s="28"/>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A185" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B185" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C185" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D185" s="22">
+        <v>47.48</v>
+      </c>
+      <c r="E185" s="14">
+        <v>2588.33</v>
+      </c>
+      <c r="F185" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
+      <c r="J185" s="1"/>
+      <c r="K185" s="1"/>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A186" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B186" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C186" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D186" s="5">
+        <v>48.88</v>
+      </c>
+      <c r="E186" s="5">
+        <v>2572.44</v>
+      </c>
+      <c r="F186" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A187" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B187" s="10">
+        <v>45072</v>
+      </c>
+      <c r="C187" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D187" s="5">
+        <v>48.88</v>
+      </c>
+      <c r="E187" s="5">
+        <v>2566.77</v>
+      </c>
+      <c r="F187" s="21" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>